<commit_message>
Updated expression evaluator to always use $ctx for context variables to eliminate conflict with source variables Added Excel based lookup loading. Added auto excel lookup generator from json lookups Updated Lookup model to include system for each lookup value. Added ExcelUtils.java and moved all excel helper methods
</commit_message>
<xml_diff>
--- a/fhir-mapper-core/mappings/excel/all-mappings.xlsx
+++ b/fhir-mapper-core/mappings/excel/all-mappings.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pradeep\POC and Experiments\Projects\fhir-mapper\fhir-mapper-core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pradeep\POC and Experiments\Projects\fhir-mapper\fhir-mapper-core\mappings\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B14DB52-684E-4005-88CC-2660520256C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A562F9E-4CB2-4C62-A6EC-F931129570E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
     <sheet name="Complex Patient JSON to FHIR Ma" sheetId="2" r:id="rId2"/>
-    <sheet name="Patient FHIR to JSON Mapping" sheetId="3" r:id="rId3"/>
-    <sheet name="Patient JSON to FHIR Mapping" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Patient FHIR to JSON Mapping" sheetId="3" r:id="rId4"/>
+    <sheet name="Patient JSON to FHIR Mapping" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="227">
   <si>
     <t>Common configuration for all mappings in this workbook</t>
   </si>
@@ -613,12 +614,6 @@
     <t>managingOrganization.reference</t>
   </si>
   <si>
-    <t>fn.concat('Organization/', organizationId)</t>
-  </si>
-  <si>
-    <t>organizationId != null</t>
-  </si>
-  <si>
     <t>FHIR_TO_JSON</t>
   </si>
   <si>
@@ -698,6 +693,18 @@
   </si>
   <si>
     <t>patient-json-to-fhir</t>
+  </si>
+  <si>
+    <t>fn.concat('Organization/', $ctx.organizationId)</t>
+  </si>
+  <si>
+    <t>complex-patient-v2</t>
+  </si>
+  <si>
+    <t>fn.concat('Organization/', $ctx.mrnSystem)</t>
+  </si>
+  <si>
+    <t>$ctx.mrnSystem != null</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1250,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1259,7 @@
     <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="63.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
@@ -1262,10 +1269,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2951,10 +2958,10 @@
         <v>35</v>
       </c>
       <c r="E53" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="F53" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="G53" t="s">
         <v>11</v>
@@ -2978,6 +2985,135 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB254AD-BB6B-449C-A22C-99A439A390B7}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -3001,10 +3137,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" t="s">
         <v>221</v>
-      </c>
-      <c r="B1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3012,7 +3148,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3028,7 +3164,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3068,7 +3204,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -3103,7 +3239,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B8" t="s">
         <v>67</v>
@@ -3138,7 +3274,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
@@ -3173,7 +3309,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B10" t="s">
         <v>80</v>
@@ -3200,15 +3336,15 @@
         <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
         <v>84</v>
@@ -3238,42 +3374,42 @@
         <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B12" t="s">
         <v>195</v>
       </c>
       <c r="C12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
       </c>
       <c r="E12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
         <v>210</v>
-      </c>
-      <c r="F12" t="s">
-        <v>211</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3281,11 +3417,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3303,10 +3439,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3322,7 +3458,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3370,7 +3506,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -3405,7 +3541,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -3429,7 +3565,7 @@
         <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -3475,7 +3611,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B10" t="s">
         <v>69</v>
@@ -3540,7 +3676,7 @@
         <v>81</v>
       </c>
       <c r="K11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3557,7 +3693,7 @@
         <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -3592,10 +3728,10 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added code documentation for TransformationTrace & FieldTransformationTrace.java
</commit_message>
<xml_diff>
--- a/fhir-mapper-core/mappings/excel/all-mappings.xlsx
+++ b/fhir-mapper-core/mappings/excel/all-mappings.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pradeep\POC and Experiments\Projects\fhir-mapper\fhir-mapper-core\mappings\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A562F9E-4CB2-4C62-A6EC-F931129570E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365158D0-2B2F-43A7-BF6E-0B5084844DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
-    <sheet name="Complex Patient JSON to FHIR Ma" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Patient-V1" sheetId="2" r:id="rId2"/>
+    <sheet name="Patient-V2" sheetId="5" r:id="rId3"/>
     <sheet name="Patient FHIR to JSON Mapping" sheetId="3" r:id="rId4"/>
     <sheet name="Patient JSON to FHIR Mapping" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -1249,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB254AD-BB6B-449C-A22C-99A439A390B7}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>